<commit_message>
Update Journal de travail - Tiago Santos.xlsx
</commit_message>
<xml_diff>
--- a/Journal de travail - Tiago Santos.xlsx
+++ b/Journal de travail - Tiago Santos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -56,13 +56,34 @@
     <t>Journal de travail - ICT 431/Bataille Navale</t>
   </si>
   <si>
-    <t>Use cases et Scénarios</t>
-  </si>
-  <si>
     <t>Bataille Navale/ICT 431</t>
   </si>
   <si>
-    <t>Initiation des use cases et scénarios</t>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initiation de la maquette </t>
+  </si>
+  <si>
+    <t>Draw.io</t>
+  </si>
+  <si>
+    <t>Continuation de la maquette</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>Clion</t>
+  </si>
+  <si>
+    <t>initiation MCD</t>
+  </si>
+  <si>
+    <t>MCD Fini</t>
+  </si>
+  <si>
+    <t>Initiation code bataille navale</t>
   </si>
 </sst>
 </file>
@@ -435,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,84 +516,142 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="3">
-        <v>43868</v>
+        <v>43894</v>
       </c>
       <c r="D3" s="4">
-        <v>0.5625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E3" s="4">
-        <v>0.62847222222222221</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="F3" s="4">
         <f>E3-D3</f>
-        <v>6.597222222222221E-2</v>
+        <v>5.9027777777777735E-2</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="3">
+        <v>43894</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="F4" s="4">
         <f t="shared" ref="F4:F49" si="0">E4-D4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+        <v>0.11805555555555558</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="3">
+        <v>43896</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+        <v>3.4722222222222154E-2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="3">
+        <v>43896</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+        <v>5.9027777777777735E-2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="3">
+        <v>43896</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>

</xml_diff>